<commit_message>
Added more names to the table. Now there are 50.
</commit_message>
<xml_diff>
--- a/UsernameDatabase.xlsx
+++ b/UsernameDatabase.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdamBrauns/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdamBrauns/Desktop/Git/OnlineGradeBook/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23000" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17340" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="108">
   <si>
     <t>First Name</t>
   </si>
@@ -198,6 +198,156 @@
   </si>
   <si>
     <t>Teacher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamara </t>
+  </si>
+  <si>
+    <t>Gamble</t>
+  </si>
+  <si>
+    <t>Dustin</t>
+  </si>
+  <si>
+    <t>Phelps</t>
+  </si>
+  <si>
+    <t>Christina</t>
+  </si>
+  <si>
+    <t>Middleton</t>
+  </si>
+  <si>
+    <t>Cali</t>
+  </si>
+  <si>
+    <t>Pearson</t>
+  </si>
+  <si>
+    <t>Russell</t>
+  </si>
+  <si>
+    <t>Rowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyle </t>
+  </si>
+  <si>
+    <t>Ramos</t>
+  </si>
+  <si>
+    <t>Jayleen</t>
+  </si>
+  <si>
+    <t>McConnell</t>
+  </si>
+  <si>
+    <t>Matthias</t>
+  </si>
+  <si>
+    <t>Bruce</t>
+  </si>
+  <si>
+    <t>Marley</t>
+  </si>
+  <si>
+    <t>Mooney</t>
+  </si>
+  <si>
+    <t>Holly</t>
+  </si>
+  <si>
+    <t>Nixon</t>
+  </si>
+  <si>
+    <t>Natalie</t>
+  </si>
+  <si>
+    <t>Woods</t>
+  </si>
+  <si>
+    <t>Kristen</t>
+  </si>
+  <si>
+    <t>Duke</t>
+  </si>
+  <si>
+    <t>Cain</t>
+  </si>
+  <si>
+    <t>Jessie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melanie </t>
+  </si>
+  <si>
+    <t>Soto</t>
+  </si>
+  <si>
+    <t>Rylee</t>
+  </si>
+  <si>
+    <t>Goodman</t>
+  </si>
+  <si>
+    <t>Savannah</t>
+  </si>
+  <si>
+    <t>Velez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damion </t>
+  </si>
+  <si>
+    <t>Cooley</t>
+  </si>
+  <si>
+    <t>Kellen</t>
+  </si>
+  <si>
+    <t>Kirby</t>
+  </si>
+  <si>
+    <t>Randolph</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>Owen</t>
+  </si>
+  <si>
+    <t>Duran</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Gould</t>
+  </si>
+  <si>
+    <t>Kyra</t>
+  </si>
+  <si>
+    <t>Fox</t>
+  </si>
+  <si>
+    <t>Weber</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Boyd</t>
+  </si>
+  <si>
+    <t>Ashlie</t>
+  </si>
+  <si>
+    <t>Kent</t>
   </si>
 </sst>
 </file>
@@ -266,8 +416,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E26" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E51" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E51"/>
   <tableColumns count="5">
     <tableColumn id="1" name="First Name"/>
     <tableColumn id="2" name="Last Name"/>
@@ -544,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,7 +938,7 @@
         <v>100011</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -806,7 +956,7 @@
         <v>100012</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -824,7 +974,7 @@
         <v>100013</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -842,7 +992,7 @@
         <v>100014</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -860,7 +1010,7 @@
         <v>100015</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -878,7 +1028,7 @@
         <v>100016</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -896,7 +1046,7 @@
         <v>100017</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -914,7 +1064,7 @@
         <v>100018</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -932,7 +1082,7 @@
         <v>100019</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -950,7 +1100,7 @@
         <v>100020</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -968,7 +1118,7 @@
         <v>100021</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -986,7 +1136,7 @@
         <v>100022</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1004,7 +1154,7 @@
         <v>100023</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1022,6 +1172,456 @@
         <v>100024</v>
       </c>
       <c r="E26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="str">
+        <f>CONCATENATE(A27,B27)</f>
+        <v>Tamara Gamble</v>
+      </c>
+      <c r="D27">
+        <v>100025</v>
+      </c>
+      <c r="E27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="str">
+        <f>CONCATENATE(A28,B28)</f>
+        <v>DustinPhelps</v>
+      </c>
+      <c r="D28">
+        <v>100026</v>
+      </c>
+      <c r="E28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" t="str">
+        <f>CONCATENATE(A29,B29)</f>
+        <v>ChristinaMiddleton</v>
+      </c>
+      <c r="D29">
+        <v>100027</v>
+      </c>
+      <c r="E29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="str">
+        <f>CONCATENATE(A30,B30)</f>
+        <v>CaliPearson</v>
+      </c>
+      <c r="D30">
+        <v>100028</v>
+      </c>
+      <c r="E30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="str">
+        <f>CONCATENATE(A31,B31)</f>
+        <v>RussellRowe</v>
+      </c>
+      <c r="D31">
+        <v>100029</v>
+      </c>
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="str">
+        <f>CONCATENATE(A32,B32)</f>
+        <v>Kyle Ramos</v>
+      </c>
+      <c r="D32">
+        <v>100030</v>
+      </c>
+      <c r="E32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="str">
+        <f>CONCATENATE(A33,B33)</f>
+        <v>JayleenMcConnell</v>
+      </c>
+      <c r="D33">
+        <v>100031</v>
+      </c>
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" t="str">
+        <f>CONCATENATE(A34,B34)</f>
+        <v>MatthiasBruce</v>
+      </c>
+      <c r="D34">
+        <v>100032</v>
+      </c>
+      <c r="E34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" t="str">
+        <f>CONCATENATE(A35,B35)</f>
+        <v>MarleyMooney</v>
+      </c>
+      <c r="D35">
+        <v>100033</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="str">
+        <f>CONCATENATE(A36,B36)</f>
+        <v>HollyNixon</v>
+      </c>
+      <c r="D36">
+        <v>100034</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" t="str">
+        <f>CONCATENATE(A37,B37)</f>
+        <v>NatalieWoods</v>
+      </c>
+      <c r="D37">
+        <v>100035</v>
+      </c>
+      <c r="E37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" t="str">
+        <f>CONCATENATE(A38,B38)</f>
+        <v>JessieCain</v>
+      </c>
+      <c r="D38">
+        <v>100036</v>
+      </c>
+      <c r="E38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" t="str">
+        <f>CONCATENATE(A39,B39)</f>
+        <v>KristenDuke</v>
+      </c>
+      <c r="D39">
+        <v>100037</v>
+      </c>
+      <c r="E39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" t="str">
+        <f>CONCATENATE(A40,B40)</f>
+        <v>Melanie Soto</v>
+      </c>
+      <c r="D40">
+        <v>100038</v>
+      </c>
+      <c r="E40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" t="str">
+        <f>CONCATENATE(A41,B41)</f>
+        <v>RyleeGoodman</v>
+      </c>
+      <c r="D41">
+        <v>100039</v>
+      </c>
+      <c r="E41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="str">
+        <f>CONCATENATE(A42,B42)</f>
+        <v>SavannahVelez</v>
+      </c>
+      <c r="D42">
+        <v>100040</v>
+      </c>
+      <c r="E42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" t="str">
+        <f>CONCATENATE(A43,B43)</f>
+        <v>Damion Cooley</v>
+      </c>
+      <c r="D43">
+        <v>100041</v>
+      </c>
+      <c r="E43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" t="str">
+        <f>CONCATENATE(A44,B44)</f>
+        <v>KellenKirby</v>
+      </c>
+      <c r="D44">
+        <v>100042</v>
+      </c>
+      <c r="E44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" t="str">
+        <f>CONCATENATE(A45,B45)</f>
+        <v>DrakeRandolph</v>
+      </c>
+      <c r="D45">
+        <v>100043</v>
+      </c>
+      <c r="E45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" t="str">
+        <f>CONCATENATE(A46,B46)</f>
+        <v>OwenDuran</v>
+      </c>
+      <c r="D46">
+        <v>100044</v>
+      </c>
+      <c r="E46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" t="str">
+        <f>CONCATENATE(A47,B47)</f>
+        <v>PatrickGould</v>
+      </c>
+      <c r="D47">
+        <v>100045</v>
+      </c>
+      <c r="E47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" t="str">
+        <f>CONCATENATE(A48,B48)</f>
+        <v>KyraFox</v>
+      </c>
+      <c r="D48">
+        <v>100046</v>
+      </c>
+      <c r="E48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" t="str">
+        <f>CONCATENATE(A49,B49)</f>
+        <v>EthanWeber</v>
+      </c>
+      <c r="D49">
+        <v>100047</v>
+      </c>
+      <c r="E49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" t="str">
+        <f>CONCATENATE(A50,B50)</f>
+        <v>MarieBoyd</v>
+      </c>
+      <c r="D50">
+        <v>100048</v>
+      </c>
+      <c r="E50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="str">
+        <f>CONCATENATE(A51,B51)</f>
+        <v>AshlieKent</v>
+      </c>
+      <c r="D51">
+        <v>100049</v>
+      </c>
+      <c r="E51" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>